<commit_message>
BOM changes to reflect the now missing 2 buttons
</commit_message>
<xml_diff>
--- a/abqmmf2018.xlsx
+++ b/abqmmf2018.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t xml:space="preserve">Part</t>
   </si>
@@ -152,12 +152,6 @@
   </si>
   <si>
     <t xml:space="preserve">S3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S5</t>
   </si>
   <si>
     <t xml:space="preserve">U$3</t>
@@ -193,6 +187,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -274,10 +269,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -517,76 +512,30 @@
         <v>44</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="D15" s="0" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>